<commit_message>
Visualisation des Données terminée
</commit_message>
<xml_diff>
--- a/res/classement_PCSI.xlsx
+++ b/res/classement_PCSI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibault/Documents/Generation_PREPA/classement_cpge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibault/Documents/Generation_PREPA/classement_cpge/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA08ADF3-07D3-7E4D-879C-2646C2C7DB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEF337C-E4F7-5643-BF4D-E9F34B26FE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="26660" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,11 +553,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,7 +900,7 @@
   <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="H2" sqref="H2:H137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -969,8 +970,8 @@
       <c r="G2">
         <v>47</v>
       </c>
-      <c r="H2">
-        <v>16.958333333333329</v>
+      <c r="H2" s="2">
+        <v>16.96</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1001,8 +1002,8 @@
       <c r="G3">
         <v>85</v>
       </c>
-      <c r="H3">
-        <v>16.954022988505749</v>
+      <c r="H3" s="2">
+        <v>16.95</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -1033,8 +1034,8 @@
       <c r="G4">
         <v>121</v>
       </c>
-      <c r="H4">
-        <v>16.951612903225811</v>
+      <c r="H4" s="2">
+        <v>16.95</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -1065,8 +1066,8 @@
       <c r="G5">
         <v>131</v>
       </c>
-      <c r="H5">
-        <v>16.92647058823529</v>
+      <c r="H5" s="2">
+        <v>16.93</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -1097,8 +1098,8 @@
       <c r="G6">
         <v>127</v>
       </c>
-      <c r="H6">
-        <v>16.826086956521738</v>
+      <c r="H6" s="2">
+        <v>16.829999999999998</v>
       </c>
       <c r="I6">
         <v>5</v>
@@ -1129,7 +1130,7 @@
       <c r="G7">
         <v>42</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>16.75</v>
       </c>
       <c r="I7">
@@ -1161,8 +1162,8 @@
       <c r="G8">
         <v>202</v>
       </c>
-      <c r="H8">
-        <v>16.679324894514771</v>
+      <c r="H8" s="2">
+        <v>16.68</v>
       </c>
       <c r="I8">
         <v>7</v>
@@ -1193,8 +1194,8 @@
       <c r="G9">
         <v>73</v>
       </c>
-      <c r="H9">
-        <v>16.64044943820225</v>
+      <c r="H9" s="2">
+        <v>16.64</v>
       </c>
       <c r="I9">
         <v>8</v>
@@ -1225,8 +1226,8 @@
       <c r="G10">
         <v>71</v>
       </c>
-      <c r="H10">
-        <v>16.627906976744189</v>
+      <c r="H10" s="2">
+        <v>16.63</v>
       </c>
       <c r="I10">
         <v>9</v>
@@ -1257,8 +1258,8 @@
       <c r="G11">
         <v>73</v>
       </c>
-      <c r="H11">
-        <v>16.62222222222222</v>
+      <c r="H11" s="2">
+        <v>16.62</v>
       </c>
       <c r="I11">
         <v>10</v>
@@ -1289,8 +1290,8 @@
       <c r="G12">
         <v>72</v>
       </c>
-      <c r="H12">
-        <v>16.4375</v>
+      <c r="H12" s="2">
+        <v>16.440000000000001</v>
       </c>
       <c r="I12">
         <v>11</v>
@@ -1321,8 +1322,8 @@
       <c r="G13">
         <v>102</v>
       </c>
-      <c r="H13">
-        <v>16.434782608695649</v>
+      <c r="H13" s="2">
+        <v>16.43</v>
       </c>
       <c r="I13">
         <v>12</v>
@@ -1353,8 +1354,8 @@
       <c r="G14">
         <v>69</v>
       </c>
-      <c r="H14">
-        <v>16.41935483870968</v>
+      <c r="H14" s="2">
+        <v>16.420000000000002</v>
       </c>
       <c r="I14">
         <v>13</v>
@@ -1385,8 +1386,8 @@
       <c r="G15">
         <v>87</v>
       </c>
-      <c r="H15">
-        <v>16.403225806451609</v>
+      <c r="H15" s="2">
+        <v>16.399999999999999</v>
       </c>
       <c r="I15">
         <v>14</v>
@@ -1417,8 +1418,8 @@
       <c r="G16">
         <v>71</v>
       </c>
-      <c r="H16">
-        <v>16.353535353535349</v>
+      <c r="H16" s="2">
+        <v>16.350000000000001</v>
       </c>
       <c r="I16">
         <v>15</v>
@@ -1449,8 +1450,8 @@
       <c r="G17">
         <v>63</v>
       </c>
-      <c r="H17">
-        <v>16.349397590361441</v>
+      <c r="H17" s="2">
+        <v>16.350000000000001</v>
       </c>
       <c r="I17">
         <v>16</v>
@@ -1481,8 +1482,8 @@
       <c r="G18">
         <v>66</v>
       </c>
-      <c r="H18">
-        <v>16.333333333333329</v>
+      <c r="H18" s="2">
+        <v>16.329999999999998</v>
       </c>
       <c r="I18">
         <v>17</v>
@@ -1513,8 +1514,8 @@
       <c r="G19">
         <v>26</v>
       </c>
-      <c r="H19">
-        <v>16.18181818181818</v>
+      <c r="H19" s="2">
+        <v>16.18</v>
       </c>
       <c r="I19">
         <v>18</v>
@@ -1545,8 +1546,8 @@
       <c r="G20">
         <v>87</v>
       </c>
-      <c r="H20">
-        <v>16.142857142857139</v>
+      <c r="H20" s="2">
+        <v>16.14</v>
       </c>
       <c r="I20">
         <v>19</v>
@@ -1577,8 +1578,8 @@
       <c r="G21">
         <v>85</v>
       </c>
-      <c r="H21">
-        <v>16.11428571428571</v>
+      <c r="H21" s="2">
+        <v>16.11</v>
       </c>
       <c r="I21">
         <v>20</v>
@@ -1609,8 +1610,8 @@
       <c r="G22">
         <v>26</v>
       </c>
-      <c r="H22">
-        <v>16.111111111111111</v>
+      <c r="H22" s="2">
+        <v>16.11</v>
       </c>
       <c r="I22">
         <v>21</v>
@@ -1641,8 +1642,8 @@
       <c r="G23">
         <v>78</v>
       </c>
-      <c r="H23">
-        <v>16.107692307692311</v>
+      <c r="H23" s="2">
+        <v>16.11</v>
       </c>
       <c r="I23">
         <v>22</v>
@@ -1673,8 +1674,8 @@
       <c r="G24">
         <v>55</v>
       </c>
-      <c r="H24">
-        <v>16.085106382978719</v>
+      <c r="H24" s="2">
+        <v>16.09</v>
       </c>
       <c r="I24">
         <v>23</v>
@@ -1705,8 +1706,8 @@
       <c r="G25">
         <v>40</v>
       </c>
-      <c r="H25">
-        <v>16.083333333333329</v>
+      <c r="H25" s="2">
+        <v>16.079999999999998</v>
       </c>
       <c r="I25">
         <v>25</v>
@@ -1737,8 +1738,8 @@
       <c r="G26">
         <v>28</v>
       </c>
-      <c r="H26">
-        <v>16.083333333333329</v>
+      <c r="H26" s="2">
+        <v>16.079999999999998</v>
       </c>
       <c r="I26">
         <v>25</v>
@@ -1769,8 +1770,8 @@
       <c r="G27">
         <v>75</v>
       </c>
-      <c r="H27">
-        <v>15.96402877697842</v>
+      <c r="H27" s="2">
+        <v>15.96</v>
       </c>
       <c r="I27">
         <v>26</v>
@@ -1801,8 +1802,8 @@
       <c r="G28">
         <v>14</v>
       </c>
-      <c r="H28">
-        <v>15.928571428571431</v>
+      <c r="H28" s="2">
+        <v>15.93</v>
       </c>
       <c r="I28">
         <v>27</v>
@@ -1833,8 +1834,8 @@
       <c r="G29">
         <v>65</v>
       </c>
-      <c r="H29">
-        <v>15.92682926829268</v>
+      <c r="H29" s="2">
+        <v>15.93</v>
       </c>
       <c r="I29">
         <v>28</v>
@@ -1865,8 +1866,8 @@
       <c r="G30">
         <v>53</v>
       </c>
-      <c r="H30">
-        <v>15.92631578947368</v>
+      <c r="H30" s="2">
+        <v>15.93</v>
       </c>
       <c r="I30">
         <v>29</v>
@@ -1897,8 +1898,8 @@
       <c r="G31">
         <v>48</v>
       </c>
-      <c r="H31">
-        <v>15.90909090909091</v>
+      <c r="H31" s="2">
+        <v>15.91</v>
       </c>
       <c r="I31">
         <v>30</v>
@@ -1929,8 +1930,8 @@
       <c r="G32">
         <v>68</v>
       </c>
-      <c r="H32">
-        <v>15.87591240875912</v>
+      <c r="H32" s="2">
+        <v>15.88</v>
       </c>
       <c r="I32">
         <v>31</v>
@@ -1961,8 +1962,8 @@
       <c r="G33">
         <v>25</v>
       </c>
-      <c r="H33">
-        <v>15.875</v>
+      <c r="H33" s="2">
+        <v>15.88</v>
       </c>
       <c r="I33">
         <v>32</v>
@@ -1993,8 +1994,8 @@
       <c r="G34">
         <v>27</v>
       </c>
-      <c r="H34">
-        <v>15.851063829787231</v>
+      <c r="H34" s="2">
+        <v>15.85</v>
       </c>
       <c r="I34">
         <v>33</v>
@@ -2025,8 +2026,8 @@
       <c r="G35">
         <v>51</v>
       </c>
-      <c r="H35">
-        <v>15.850574712643679</v>
+      <c r="H35" s="2">
+        <v>15.85</v>
       </c>
       <c r="I35">
         <v>34</v>
@@ -2057,8 +2058,8 @@
       <c r="G36">
         <v>45</v>
       </c>
-      <c r="H36">
-        <v>15.712643678160919</v>
+      <c r="H36" s="2">
+        <v>15.71</v>
       </c>
       <c r="I36">
         <v>35</v>
@@ -2089,8 +2090,8 @@
       <c r="G37">
         <v>10</v>
       </c>
-      <c r="H37">
-        <v>15.69230769230769</v>
+      <c r="H37" s="2">
+        <v>15.69</v>
       </c>
       <c r="I37">
         <v>36</v>
@@ -2121,8 +2122,8 @@
       <c r="G38">
         <v>41</v>
       </c>
-      <c r="H38">
-        <v>15.638297872340431</v>
+      <c r="H38" s="2">
+        <v>15.64</v>
       </c>
       <c r="I38">
         <v>37</v>
@@ -2153,8 +2154,8 @@
       <c r="G39">
         <v>22</v>
       </c>
-      <c r="H39">
-        <v>15.62222222222222</v>
+      <c r="H39" s="2">
+        <v>15.62</v>
       </c>
       <c r="I39">
         <v>38</v>
@@ -2185,8 +2186,8 @@
       <c r="G40">
         <v>12</v>
       </c>
-      <c r="H40">
-        <v>15.52941176470588</v>
+      <c r="H40" s="2">
+        <v>15.53</v>
       </c>
       <c r="I40">
         <v>39</v>
@@ -2217,8 +2218,8 @@
       <c r="G41">
         <v>32</v>
       </c>
-      <c r="H41">
-        <v>15.3956043956044</v>
+      <c r="H41" s="2">
+        <v>15.4</v>
       </c>
       <c r="I41">
         <v>40</v>
@@ -2249,8 +2250,8 @@
       <c r="G42">
         <v>8</v>
       </c>
-      <c r="H42">
-        <v>15.36363636363636</v>
+      <c r="H42" s="2">
+        <v>15.36</v>
       </c>
       <c r="I42">
         <v>41</v>
@@ -2281,8 +2282,8 @@
       <c r="G43">
         <v>14</v>
       </c>
-      <c r="H43">
-        <v>15.34782608695652</v>
+      <c r="H43" s="2">
+        <v>15.35</v>
       </c>
       <c r="I43">
         <v>42</v>
@@ -2313,8 +2314,8 @@
       <c r="G44">
         <v>32</v>
       </c>
-      <c r="H44">
-        <v>15.340425531914891</v>
+      <c r="H44" s="2">
+        <v>15.34</v>
       </c>
       <c r="I44">
         <v>43</v>
@@ -2345,8 +2346,8 @@
       <c r="G45">
         <v>1</v>
       </c>
-      <c r="H45">
-        <v>15.31818181818182</v>
+      <c r="H45" s="2">
+        <v>15.32</v>
       </c>
       <c r="I45">
         <v>45</v>
@@ -2377,8 +2378,8 @@
       <c r="G46">
         <v>15</v>
       </c>
-      <c r="H46">
-        <v>15.31818181818182</v>
+      <c r="H46" s="2">
+        <v>15.32</v>
       </c>
       <c r="I46">
         <v>45</v>
@@ -2409,8 +2410,8 @@
       <c r="G47">
         <v>14</v>
       </c>
-      <c r="H47">
-        <v>15.297872340425529</v>
+      <c r="H47" s="2">
+        <v>15.3</v>
       </c>
       <c r="I47">
         <v>46</v>
@@ -2441,8 +2442,8 @@
       <c r="G48">
         <v>14</v>
       </c>
-      <c r="H48">
-        <v>15.238095238095241</v>
+      <c r="H48" s="2">
+        <v>15.24</v>
       </c>
       <c r="I48">
         <v>47</v>
@@ -2473,8 +2474,8 @@
       <c r="G49">
         <v>8</v>
       </c>
-      <c r="H49">
-        <v>15.23076923076923</v>
+      <c r="H49" s="2">
+        <v>15.23</v>
       </c>
       <c r="I49">
         <v>48</v>
@@ -2505,8 +2506,8 @@
       <c r="G50">
         <v>12</v>
       </c>
-      <c r="H50">
-        <v>15.163265306122449</v>
+      <c r="H50" s="2">
+        <v>15.16</v>
       </c>
       <c r="I50">
         <v>49</v>
@@ -2537,8 +2538,8 @@
       <c r="G51">
         <v>26</v>
       </c>
-      <c r="H51">
-        <v>15.147368421052629</v>
+      <c r="H51" s="2">
+        <v>15.15</v>
       </c>
       <c r="I51">
         <v>50</v>
@@ -2569,8 +2570,8 @@
       <c r="G52">
         <v>13</v>
       </c>
-      <c r="H52">
-        <v>15.06451612903226</v>
+      <c r="H52" s="2">
+        <v>15.06</v>
       </c>
       <c r="I52">
         <v>51</v>
@@ -2601,8 +2602,8 @@
       <c r="G53">
         <v>49</v>
       </c>
-      <c r="H53">
-        <v>15.06451612903226</v>
+      <c r="H53" s="2">
+        <v>15.06</v>
       </c>
       <c r="I53">
         <v>53</v>
@@ -2633,8 +2634,8 @@
       <c r="G54">
         <v>10</v>
       </c>
-      <c r="H54">
-        <v>15.06451612903226</v>
+      <c r="H54" s="2">
+        <v>15.06</v>
       </c>
       <c r="I54">
         <v>53</v>
@@ -2665,7 +2666,7 @@
       <c r="G55">
         <v>16</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="2">
         <v>15</v>
       </c>
       <c r="I55">
@@ -2697,7 +2698,7 @@
       <c r="G56">
         <v>21</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="2">
         <v>15</v>
       </c>
       <c r="I56">
@@ -2729,8 +2730,8 @@
       <c r="G57">
         <v>12</v>
       </c>
-      <c r="H57">
-        <v>14.95121951219512</v>
+      <c r="H57" s="2">
+        <v>14.95</v>
       </c>
       <c r="I57">
         <v>56</v>
@@ -2761,8 +2762,8 @@
       <c r="G58">
         <v>11</v>
       </c>
-      <c r="H58">
-        <v>14.945945945945949</v>
+      <c r="H58" s="2">
+        <v>14.95</v>
       </c>
       <c r="I58">
         <v>57</v>
@@ -2793,8 +2794,8 @@
       <c r="G59">
         <v>25</v>
       </c>
-      <c r="H59">
-        <v>14.90476190476191</v>
+      <c r="H59" s="2">
+        <v>14.9</v>
       </c>
       <c r="I59">
         <v>58</v>
@@ -2825,8 +2826,8 @@
       <c r="G60">
         <v>10</v>
       </c>
-      <c r="H60">
-        <v>14.891891891891889</v>
+      <c r="H60" s="2">
+        <v>14.89</v>
       </c>
       <c r="I60">
         <v>59</v>
@@ -2857,8 +2858,8 @@
       <c r="G61">
         <v>9</v>
       </c>
-      <c r="H61">
-        <v>14.86363636363636</v>
+      <c r="H61" s="2">
+        <v>14.86</v>
       </c>
       <c r="I61">
         <v>60</v>
@@ -2889,8 +2890,8 @@
       <c r="G62">
         <v>31</v>
       </c>
-      <c r="H62">
-        <v>14.838709677419351</v>
+      <c r="H62" s="2">
+        <v>14.84</v>
       </c>
       <c r="I62">
         <v>62</v>
@@ -2921,8 +2922,8 @@
       <c r="G63">
         <v>17</v>
       </c>
-      <c r="H63">
-        <v>14.838709677419351</v>
+      <c r="H63" s="2">
+        <v>14.84</v>
       </c>
       <c r="I63">
         <v>62</v>
@@ -2953,8 +2954,8 @@
       <c r="G64">
         <v>6</v>
       </c>
-      <c r="H64">
-        <v>14.82608695652174</v>
+      <c r="H64" s="2">
+        <v>14.83</v>
       </c>
       <c r="I64">
         <v>63</v>
@@ -2985,7 +2986,7 @@
       <c r="G65">
         <v>9</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="2">
         <v>14.75</v>
       </c>
       <c r="I65">
@@ -3017,8 +3018,8 @@
       <c r="G66">
         <v>12</v>
       </c>
-      <c r="H66">
-        <v>14.72972972972973</v>
+      <c r="H66" s="2">
+        <v>14.73</v>
       </c>
       <c r="I66">
         <v>65</v>
@@ -3049,8 +3050,8 @@
       <c r="G67">
         <v>16</v>
       </c>
-      <c r="H67">
-        <v>14.71830985915493</v>
+      <c r="H67" s="2">
+        <v>14.72</v>
       </c>
       <c r="I67">
         <v>66</v>
@@ -3081,8 +3082,8 @@
       <c r="G68">
         <v>9</v>
       </c>
-      <c r="H68">
-        <v>14.69230769230769</v>
+      <c r="H68" s="2">
+        <v>14.69</v>
       </c>
       <c r="I68">
         <v>67</v>
@@ -3113,8 +3114,8 @@
       <c r="G69">
         <v>9</v>
       </c>
-      <c r="H69">
-        <v>14.68181818181818</v>
+      <c r="H69" s="2">
+        <v>14.68</v>
       </c>
       <c r="I69">
         <v>68</v>
@@ -3145,8 +3146,8 @@
       <c r="G70">
         <v>8</v>
       </c>
-      <c r="H70">
-        <v>14.64444444444444</v>
+      <c r="H70" s="2">
+        <v>14.64</v>
       </c>
       <c r="I70">
         <v>69</v>
@@ -3177,8 +3178,8 @@
       <c r="G71">
         <v>4</v>
       </c>
-      <c r="H71">
-        <v>14.63636363636364</v>
+      <c r="H71" s="2">
+        <v>14.64</v>
       </c>
       <c r="I71">
         <v>70</v>
@@ -3209,8 +3210,8 @@
       <c r="G72">
         <v>38</v>
       </c>
-      <c r="H72">
-        <v>14.631578947368419</v>
+      <c r="H72" s="2">
+        <v>14.63</v>
       </c>
       <c r="I72">
         <v>72</v>
@@ -3241,8 +3242,8 @@
       <c r="G73">
         <v>5</v>
       </c>
-      <c r="H73">
-        <v>14.631578947368419</v>
+      <c r="H73" s="2">
+        <v>14.63</v>
       </c>
       <c r="I73">
         <v>72</v>
@@ -3273,8 +3274,8 @@
       <c r="G74">
         <v>15</v>
       </c>
-      <c r="H74">
-        <v>14.607142857142859</v>
+      <c r="H74" s="2">
+        <v>14.61</v>
       </c>
       <c r="I74">
         <v>73</v>
@@ -3305,7 +3306,7 @@
       <c r="G75">
         <v>4</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="2">
         <v>14.6</v>
       </c>
       <c r="I75">
@@ -3337,7 +3338,7 @@
       <c r="G76">
         <v>6</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="2">
         <v>14.6</v>
       </c>
       <c r="I76">
@@ -3369,8 +3370,8 @@
       <c r="G77">
         <v>21</v>
       </c>
-      <c r="H77">
-        <v>14.5959595959596</v>
+      <c r="H77" s="2">
+        <v>14.6</v>
       </c>
       <c r="I77">
         <v>76</v>
@@ -3401,8 +3402,8 @@
       <c r="G78">
         <v>12</v>
       </c>
-      <c r="H78">
-        <v>14.57894736842105</v>
+      <c r="H78" s="2">
+        <v>14.58</v>
       </c>
       <c r="I78">
         <v>77</v>
@@ -3433,8 +3434,8 @@
       <c r="G79">
         <v>16</v>
       </c>
-      <c r="H79">
-        <v>14.54929577464789</v>
+      <c r="H79" s="2">
+        <v>14.55</v>
       </c>
       <c r="I79">
         <v>78</v>
@@ -3465,8 +3466,8 @@
       <c r="G80">
         <v>20</v>
       </c>
-      <c r="H80">
-        <v>14.494505494505489</v>
+      <c r="H80" s="2">
+        <v>14.49</v>
       </c>
       <c r="I80">
         <v>79</v>
@@ -3497,8 +3498,8 @@
       <c r="G81">
         <v>3</v>
       </c>
-      <c r="H81">
-        <v>14.487179487179491</v>
+      <c r="H81" s="2">
+        <v>14.49</v>
       </c>
       <c r="I81">
         <v>81</v>
@@ -3529,8 +3530,8 @@
       <c r="G82">
         <v>7</v>
       </c>
-      <c r="H82">
-        <v>14.487179487179491</v>
+      <c r="H82" s="2">
+        <v>14.49</v>
       </c>
       <c r="I82">
         <v>81</v>
@@ -3561,8 +3562,8 @@
       <c r="G83">
         <v>8</v>
       </c>
-      <c r="H83">
-        <v>14.43589743589744</v>
+      <c r="H83" s="2">
+        <v>14.44</v>
       </c>
       <c r="I83">
         <v>82</v>
@@ -3593,8 +3594,8 @@
       <c r="G84">
         <v>6</v>
       </c>
-      <c r="H84">
-        <v>14.434782608695651</v>
+      <c r="H84" s="2">
+        <v>14.43</v>
       </c>
       <c r="I84">
         <v>83</v>
@@ -3625,8 +3626,8 @@
       <c r="G85">
         <v>7</v>
       </c>
-      <c r="H85">
-        <v>14.38461538461539</v>
+      <c r="H85" s="2">
+        <v>14.38</v>
       </c>
       <c r="I85">
         <v>84</v>
@@ -3657,8 +3658,8 @@
       <c r="G86">
         <v>8</v>
       </c>
-      <c r="H86">
-        <v>14.34883720930233</v>
+      <c r="H86" s="2">
+        <v>14.35</v>
       </c>
       <c r="I86">
         <v>85</v>
@@ -3689,8 +3690,8 @@
       <c r="G87">
         <v>2</v>
       </c>
-      <c r="H87">
-        <v>14.27272727272727</v>
+      <c r="H87" s="2">
+        <v>14.27</v>
       </c>
       <c r="I87">
         <v>86</v>
@@ -3721,8 +3722,8 @@
       <c r="G88">
         <v>7</v>
       </c>
-      <c r="H88">
-        <v>14.24324324324324</v>
+      <c r="H88" s="2">
+        <v>14.24</v>
       </c>
       <c r="I88">
         <v>87</v>
@@ -3753,8 +3754,8 @@
       <c r="G89">
         <v>12</v>
       </c>
-      <c r="H89">
-        <v>14.23076923076923</v>
+      <c r="H89" s="2">
+        <v>14.23</v>
       </c>
       <c r="I89">
         <v>88</v>
@@ -3785,8 +3786,8 @@
       <c r="G90">
         <v>1</v>
       </c>
-      <c r="H90">
-        <v>14.23076923076923</v>
+      <c r="H90" s="2">
+        <v>14.23</v>
       </c>
       <c r="I90">
         <v>89</v>
@@ -3817,8 +3818,8 @@
       <c r="G91">
         <v>2</v>
       </c>
-      <c r="H91">
-        <v>14.18181818181818</v>
+      <c r="H91" s="2">
+        <v>14.18</v>
       </c>
       <c r="I91">
         <v>90</v>
@@ -3849,8 +3850,8 @@
       <c r="G92">
         <v>4</v>
       </c>
-      <c r="H92">
-        <v>14.17241379310345</v>
+      <c r="H92" s="2">
+        <v>14.17</v>
       </c>
       <c r="I92">
         <v>91</v>
@@ -3881,8 +3882,8 @@
       <c r="G93">
         <v>7</v>
       </c>
-      <c r="H93">
-        <v>14.16666666666667</v>
+      <c r="H93" s="2">
+        <v>14.17</v>
       </c>
       <c r="I93">
         <v>92</v>
@@ -3913,8 +3914,8 @@
       <c r="G94">
         <v>6</v>
       </c>
-      <c r="H94">
-        <v>14.125</v>
+      <c r="H94" s="2">
+        <v>14.13</v>
       </c>
       <c r="I94">
         <v>93</v>
@@ -3945,8 +3946,8 @@
       <c r="G95">
         <v>13</v>
       </c>
-      <c r="H95">
-        <v>14.09375</v>
+      <c r="H95" s="2">
+        <v>14.09</v>
       </c>
       <c r="I95">
         <v>94</v>
@@ -3977,8 +3978,8 @@
       <c r="G96">
         <v>6</v>
       </c>
-      <c r="H96">
-        <v>14.09090909090909</v>
+      <c r="H96" s="2">
+        <v>14.09</v>
       </c>
       <c r="I96">
         <v>95</v>
@@ -4009,8 +4010,8 @@
       <c r="G97">
         <v>2</v>
       </c>
-      <c r="H97">
-        <v>14.085714285714291</v>
+      <c r="H97" s="2">
+        <v>14.09</v>
       </c>
       <c r="I97">
         <v>96</v>
@@ -4041,8 +4042,8 @@
       <c r="G98">
         <v>5</v>
       </c>
-      <c r="H98">
-        <v>14.069767441860471</v>
+      <c r="H98" s="2">
+        <v>14.07</v>
       </c>
       <c r="I98">
         <v>97</v>
@@ -4073,8 +4074,8 @@
       <c r="G99">
         <v>4</v>
       </c>
-      <c r="H99">
-        <v>14.05263157894737</v>
+      <c r="H99" s="2">
+        <v>14.05</v>
       </c>
       <c r="I99">
         <v>98</v>
@@ -4105,8 +4106,8 @@
       <c r="G100">
         <v>4</v>
       </c>
-      <c r="H100">
-        <v>14.03703703703704</v>
+      <c r="H100" s="2">
+        <v>14.04</v>
       </c>
       <c r="I100">
         <v>99</v>
@@ -4137,7 +4138,7 @@
       <c r="G101">
         <v>1</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="2">
         <v>14</v>
       </c>
       <c r="I101">
@@ -4169,7 +4170,7 @@
       <c r="G102">
         <v>3</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="2">
         <v>14</v>
       </c>
       <c r="I102">
@@ -4201,8 +4202,8 @@
       <c r="G103">
         <v>3</v>
       </c>
-      <c r="H103">
-        <v>13.86363636363636</v>
+      <c r="H103" s="2">
+        <v>13.86</v>
       </c>
       <c r="I103">
         <v>102</v>
@@ -4233,8 +4234,8 @@
       <c r="G104">
         <v>1</v>
       </c>
-      <c r="H104">
-        <v>13.83333333333333</v>
+      <c r="H104" s="2">
+        <v>13.83</v>
       </c>
       <c r="I104">
         <v>103</v>
@@ -4265,8 +4266,8 @@
       <c r="G105">
         <v>2</v>
       </c>
-      <c r="H105">
-        <v>13.83333333333333</v>
+      <c r="H105" s="2">
+        <v>13.83</v>
       </c>
       <c r="I105">
         <v>104</v>
@@ -4297,8 +4298,8 @@
       <c r="G106">
         <v>5</v>
       </c>
-      <c r="H106">
-        <v>13.82352941176471</v>
+      <c r="H106" s="2">
+        <v>13.82</v>
       </c>
       <c r="I106">
         <v>105</v>
@@ -4329,7 +4330,7 @@
       <c r="G107">
         <v>3</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="2">
         <v>13.8</v>
       </c>
       <c r="I107">
@@ -4361,8 +4362,8 @@
       <c r="G108">
         <v>1</v>
       </c>
-      <c r="H108">
-        <v>13.74285714285714</v>
+      <c r="H108" s="2">
+        <v>13.74</v>
       </c>
       <c r="I108">
         <v>107</v>
@@ -4393,8 +4394,8 @@
       <c r="G109">
         <v>3</v>
       </c>
-      <c r="H109">
-        <v>13.707692307692311</v>
+      <c r="H109" s="2">
+        <v>13.71</v>
       </c>
       <c r="I109">
         <v>108</v>
@@ -4425,8 +4426,8 @@
       <c r="G110">
         <v>6</v>
       </c>
-      <c r="H110">
-        <v>13.697674418604651</v>
+      <c r="H110" s="2">
+        <v>13.7</v>
       </c>
       <c r="I110">
         <v>109</v>
@@ -4457,8 +4458,8 @@
       <c r="G111">
         <v>2</v>
       </c>
-      <c r="H111">
-        <v>13.695652173913039</v>
+      <c r="H111" s="2">
+        <v>13.7</v>
       </c>
       <c r="I111">
         <v>110</v>
@@ -4489,8 +4490,8 @@
       <c r="G112">
         <v>0</v>
       </c>
-      <c r="H112">
-        <v>13.66666666666667</v>
+      <c r="H112" s="2">
+        <v>13.67</v>
       </c>
       <c r="I112">
         <v>111</v>
@@ -4521,8 +4522,8 @@
       <c r="G113">
         <v>5</v>
       </c>
-      <c r="H113">
-        <v>13.65573770491803</v>
+      <c r="H113" s="2">
+        <v>13.66</v>
       </c>
       <c r="I113">
         <v>112</v>
@@ -4553,8 +4554,8 @@
       <c r="G114">
         <v>3</v>
       </c>
-      <c r="H114">
-        <v>13.64516129032258</v>
+      <c r="H114" s="2">
+        <v>13.65</v>
       </c>
       <c r="I114">
         <v>113</v>
@@ -4585,8 +4586,8 @@
       <c r="G115">
         <v>3</v>
       </c>
-      <c r="H115">
-        <v>13.571428571428569</v>
+      <c r="H115" s="2">
+        <v>13.57</v>
       </c>
       <c r="I115">
         <v>114</v>
@@ -4617,8 +4618,8 @@
       <c r="G116">
         <v>2</v>
       </c>
-      <c r="H116">
-        <v>13.47619047619048</v>
+      <c r="H116" s="2">
+        <v>13.48</v>
       </c>
       <c r="I116">
         <v>115</v>
@@ -4649,8 +4650,8 @@
       <c r="G117">
         <v>1</v>
       </c>
-      <c r="H117">
-        <v>13.428571428571431</v>
+      <c r="H117" s="2">
+        <v>13.43</v>
       </c>
       <c r="I117">
         <v>116</v>
@@ -4681,8 +4682,8 @@
       <c r="G118">
         <v>1</v>
       </c>
-      <c r="H118">
-        <v>13.413793103448279</v>
+      <c r="H118" s="2">
+        <v>13.41</v>
       </c>
       <c r="I118">
         <v>118</v>
@@ -4713,8 +4714,8 @@
       <c r="G119">
         <v>1</v>
       </c>
-      <c r="H119">
-        <v>13.413793103448279</v>
+      <c r="H119" s="2">
+        <v>13.41</v>
       </c>
       <c r="I119">
         <v>118</v>
@@ -4745,8 +4746,8 @@
       <c r="G120">
         <v>1</v>
       </c>
-      <c r="H120">
-        <v>13.24242424242424</v>
+      <c r="H120" s="2">
+        <v>13.24</v>
       </c>
       <c r="I120">
         <v>119</v>
@@ -4777,8 +4778,8 @@
       <c r="G121">
         <v>2</v>
       </c>
-      <c r="H121">
-        <v>13.22222222222222</v>
+      <c r="H121" s="2">
+        <v>13.22</v>
       </c>
       <c r="I121">
         <v>120</v>
@@ -4809,8 +4810,8 @@
       <c r="G122">
         <v>1</v>
       </c>
-      <c r="H122">
-        <v>13.18181818181818</v>
+      <c r="H122" s="2">
+        <v>13.18</v>
       </c>
       <c r="I122">
         <v>121</v>
@@ -4841,8 +4842,8 @@
       <c r="G123">
         <v>2</v>
       </c>
-      <c r="H123">
-        <v>13.08333333333333</v>
+      <c r="H123" s="2">
+        <v>13.08</v>
       </c>
       <c r="I123">
         <v>122</v>
@@ -4873,8 +4874,8 @@
       <c r="G124">
         <v>1</v>
       </c>
-      <c r="H124">
-        <v>13.074074074074071</v>
+      <c r="H124" s="2">
+        <v>13.07</v>
       </c>
       <c r="I124">
         <v>123</v>
@@ -4905,7 +4906,7 @@
       <c r="G125">
         <v>3</v>
       </c>
-      <c r="H125">
+      <c r="H125" s="2">
         <v>13</v>
       </c>
       <c r="I125">
@@ -4937,7 +4938,7 @@
       <c r="G126">
         <v>1</v>
       </c>
-      <c r="H126">
+      <c r="H126" s="2">
         <v>13</v>
       </c>
       <c r="I126">
@@ -4969,8 +4970,8 @@
       <c r="G127">
         <v>0</v>
       </c>
-      <c r="H127">
-        <v>12.94736842105263</v>
+      <c r="H127" s="2">
+        <v>12.95</v>
       </c>
       <c r="I127">
         <v>126</v>
@@ -5001,8 +5002,8 @@
       <c r="G128">
         <v>1</v>
       </c>
-      <c r="H128">
-        <v>12.913043478260869</v>
+      <c r="H128" s="2">
+        <v>12.91</v>
       </c>
       <c r="I128">
         <v>127</v>
@@ -5033,8 +5034,8 @@
       <c r="G129">
         <v>2</v>
       </c>
-      <c r="H129">
-        <v>12.766233766233769</v>
+      <c r="H129" s="2">
+        <v>12.77</v>
       </c>
       <c r="I129">
         <v>128</v>
@@ -5065,8 +5066,8 @@
       <c r="G130">
         <v>2</v>
       </c>
-      <c r="H130">
-        <v>12.739130434782609</v>
+      <c r="H130" s="2">
+        <v>12.74</v>
       </c>
       <c r="I130">
         <v>129</v>
@@ -5097,8 +5098,8 @@
       <c r="G131">
         <v>0</v>
       </c>
-      <c r="H131">
-        <v>12.63636363636364</v>
+      <c r="H131" s="2">
+        <v>12.64</v>
       </c>
       <c r="I131">
         <v>130</v>
@@ -5129,7 +5130,7 @@
       <c r="G132">
         <v>0</v>
       </c>
-      <c r="H132">
+      <c r="H132" s="2">
         <v>12.6</v>
       </c>
       <c r="I132">
@@ -5161,8 +5162,8 @@
       <c r="G133">
         <v>0</v>
       </c>
-      <c r="H133">
-        <v>12.46153846153846</v>
+      <c r="H133" s="2">
+        <v>12.46</v>
       </c>
       <c r="I133">
         <v>132</v>
@@ -5193,7 +5194,7 @@
       <c r="G134">
         <v>1</v>
       </c>
-      <c r="H134">
+      <c r="H134" s="2">
         <v>12.44</v>
       </c>
       <c r="I134">
@@ -5225,8 +5226,8 @@
       <c r="G135">
         <v>1</v>
       </c>
-      <c r="H135">
-        <v>12.379310344827591</v>
+      <c r="H135" s="2">
+        <v>12.38</v>
       </c>
       <c r="I135">
         <v>134</v>
@@ -5257,8 +5258,8 @@
       <c r="G136">
         <v>1</v>
       </c>
-      <c r="H136">
-        <v>12.33333333333333</v>
+      <c r="H136" s="2">
+        <v>12.33</v>
       </c>
       <c r="I136">
         <v>136</v>
@@ -5289,8 +5290,8 @@
       <c r="G137">
         <v>1</v>
       </c>
-      <c r="H137">
-        <v>12.27272727272727</v>
+      <c r="H137" s="2">
+        <v>12.27</v>
       </c>
       <c r="I137">
         <v>137</v>

</xml_diff>